<commit_message>
Ec. Continuidad - 9 de enero de 2024 - Lap HP
Se actualiza el repositorio con el material de hidrodinámica.
</commit_message>
<xml_diff>
--- a/Bitacoras/Parcial_02/Bitacora_Fisica_4_02_Segundo_Parcial_Evaluacion_Continua.xlsx
+++ b/Bitacoras/Parcial_02/Bitacora_Fisica_4_02_Segundo_Parcial_Evaluacion_Continua.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusto\OneDrive\Documentos\Cursos_UVM\Plan PU\Fisica_4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusto\OneDrive\Documentos\Cursos_UVM\Plan PU\Fisica_4\Bitacoras\Parcial_02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8619CC99-0790-4316-92E5-C49491A71EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8490388-E066-4950-BF8F-CAF366F66BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{4FD94BEE-9FA1-43C4-B1A5-7667194BB0F1}"/>
   </bookViews>
@@ -2907,7 +2907,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>